<commit_message>
Add nil value read/write
</commit_message>
<xml_diff>
--- a/graph.xlsx
+++ b/graph.xlsx
@@ -1,25 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21310"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\MessagePack-CSharp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C89E4D-52EA-4D61-B931-0C492B106DB4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17AC13D5-2D3C-4ED3-92DC-73D82ACB0431}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48480" yWindow="-3600" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README graph" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -147,10 +155,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -170,13 +180,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -186,10 +197,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{EEED627A-A0C2-4276-9DBE-5120BEC3B1C1}"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3917,16 +3930,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>100013</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4344,213 +4357,364 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C478671A-2BFF-4005-AC60-F5FFFBF24A55}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="19.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.06640625" style="1"/>
+    <col min="3" max="3" width="9.53125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.06640625" style="5"/>
+    <col min="5" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="4">
         <v>137.69999999999999</v>
       </c>
+      <c r="C3" s="4">
+        <v>158.55000000000001</v>
+      </c>
+      <c r="D3" s="5">
+        <f>C3/B3</f>
+        <v>1.1514161220043575</v>
+      </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="4">
         <v>160.72999999999999</v>
       </c>
+      <c r="C4" s="4">
+        <v>221.66</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" ref="D4:D9" si="0">C4/B4</f>
+        <v>1.379082934113109</v>
+      </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="4">
         <v>335.23</v>
       </c>
+      <c r="C5" s="4">
+        <v>349.17</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" si="0"/>
+        <v>1.0415833905080094</v>
+      </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4">
         <v>449.62</v>
       </c>
+      <c r="C6" s="4">
+        <v>463.91</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" si="0"/>
+        <v>1.0317823940216182</v>
+      </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="4">
         <v>141.72999999999999</v>
       </c>
+      <c r="C7" s="4">
+        <v>144.47</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" si="0"/>
+        <v>1.0193325336908206</v>
+      </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="4">
         <v>1543.3</v>
       </c>
+      <c r="C8" s="4">
+        <v>1177.2</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.76278105358647064</v>
+      </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="4">
         <v>1680.56</v>
       </c>
+      <c r="C9" s="4">
+        <v>1872.76</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
+        <v>1.1143666396915315</v>
+      </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:4">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="4">
         <v>177.33</v>
       </c>
+      <c r="C12" s="4">
+        <v>747.22</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" ref="D12:D18" si="1">C12/B12</f>
+        <v>4.213725821913946</v>
+      </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="4">
         <v>182.04</v>
       </c>
+      <c r="C13" s="4">
+        <v>872.62</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" si="1"/>
+        <v>4.7935618545374643</v>
+      </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:4">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="4">
         <v>1106.8699999999999</v>
       </c>
+      <c r="C14" s="4">
+        <v>1364.81</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" si="1"/>
+        <v>1.2330354964901027</v>
+      </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="4">
         <v>627.23</v>
       </c>
+      <c r="C15" s="4">
+        <v>602.02</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" si="1"/>
+        <v>0.95980740717121305</v>
+      </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="4">
         <v>139.91</v>
       </c>
+      <c r="C16" s="4">
+        <v>154.31</v>
+      </c>
+      <c r="D16" s="5">
+        <f t="shared" si="1"/>
+        <v>1.1029233078407548</v>
+      </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="4">
         <v>1876.02</v>
       </c>
+      <c r="C17" s="4">
+        <v>2529.08</v>
+      </c>
+      <c r="D17" s="5">
+        <f t="shared" si="1"/>
+        <v>1.3481092952100724</v>
+      </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="4">
         <v>2237.38</v>
       </c>
+      <c r="C18" s="4">
+        <v>2705.08</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" si="1"/>
+        <v>1.2090391439987842</v>
+      </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:4">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="2">
         <v>1803</v>
       </c>
+      <c r="C21" s="2">
+        <v>1803</v>
+      </c>
+      <c r="D21" s="5">
+        <f t="shared" ref="D21:D27" si="2">C21/B21</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="2">
         <v>562</v>
       </c>
+      <c r="C22" s="2">
+        <v>562</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B23" s="2">
         <v>2347</v>
       </c>
+      <c r="C23" s="2">
+        <v>2347</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="2">
         <v>2248</v>
       </c>
+      <c r="C24" s="2">
+        <v>2248</v>
+      </c>
+      <c r="D24" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B25" s="2">
         <v>5004</v>
       </c>
+      <c r="C25" s="2">
+        <v>5004</v>
+      </c>
+      <c r="D25" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B26" s="2">
         <v>6096</v>
       </c>
+      <c r="C26" s="2">
+        <v>6096</v>
+      </c>
+      <c r="D26" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B27" s="2">
         <v>458</v>
+      </c>
+      <c r="C27" s="2">
+        <v>458</v>
+      </c>
+      <c r="D27" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>